<commit_message>
Burndown Chart Update igen
</commit_message>
<xml_diff>
--- a/Sprint Backlog 1.xlsx
+++ b/Sprint Backlog 1.xlsx
@@ -111,7 +111,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +154,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -167,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -188,6 +194,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -277,7 +286,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -350,11 +359,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="130401280"/>
-        <c:axId val="90394560"/>
+        <c:axId val="124371968"/>
+        <c:axId val="84365248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="130401280"/>
+        <c:axId val="124371968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -363,7 +372,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90394560"/>
+        <c:crossAx val="84365248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -371,7 +380,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90394560"/>
+        <c:axId val="84365248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,7 +406,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130401280"/>
+        <c:crossAx val="124371968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -736,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -838,7 +847,7 @@
         <v>4</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -892,7 +901,7 @@
         <v>4</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -921,6 +930,9 @@
       <c r="J7">
         <v>0</v>
       </c>
+    </row>
+    <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Burndown Chart är klar för den första sprinte
</commit_message>
<xml_diff>
--- a/Sprint Backlog 1.xlsx
+++ b/Sprint Backlog 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Klar</t>
-  </si>
-  <si>
-    <t>Håller på</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -359,11 +356,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="124371968"/>
-        <c:axId val="84365248"/>
+        <c:axId val="126862336"/>
+        <c:axId val="84692928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124371968"/>
+        <c:axId val="126862336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +369,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84365248"/>
+        <c:crossAx val="84692928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -380,7 +377,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84365248"/>
+        <c:axId val="84692928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +403,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124371968"/>
+        <c:crossAx val="126862336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -748,7 +745,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -837,7 +834,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3">
@@ -850,7 +847,7 @@
         <v>3</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -904,7 +901,7 @@
         <v>3</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>0</v>

</xml_diff>